<commit_message>
nats usbs added to bom
</commit_message>
<xml_diff>
--- a/Grouped_BOMs/Schrack_Grouped.xlsx
+++ b/Grouped_BOMs/Schrack_Grouped.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\MenMe\GitHub\SchrackProjects\Grouped_BOMs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{32368DCC-9B5F-4B4E-BA74-0319E0FF702C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F3842343-6070-48B2-B3ED-D5DCA8A7C647}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11020" xr2:uid="{4A963E85-4DE0-42E6-9C41-0B0E9DF7A811}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="322" uniqueCount="124">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="324" uniqueCount="126">
   <si>
     <t>Designator</t>
   </si>
@@ -408,6 +408,12 @@
   </si>
   <si>
     <t>https://cz.mouser.com/ProductDetail/Vishay-Dale/CRCW0805220RFKEAHP?qs=40TFAHZMFveaN1fEKh2bRA%3D%3D</t>
+  </si>
+  <si>
+    <t>USB - FEMALE, NAT, TME</t>
+  </si>
+  <si>
+    <t>USB - MALE, NAT, TME</t>
   </si>
 </sst>
 </file>
@@ -983,7 +989,7 @@
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="24">
+  <cellXfs count="26">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="35" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1046,6 +1052,10 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="18" fillId="33" borderId="0" xfId="42" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="33" borderId="0" xfId="42" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="33" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
@@ -1426,8 +1436,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{922EDB62-CB86-4964-8550-0065867A2EA4}">
   <dimension ref="A1:K82"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="84" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="J12" sqref="J12"/>
+    <sheetView tabSelected="1" topLeftCell="B8" zoomScale="84" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="I15" sqref="I15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1866,13 +1876,13 @@
         <f t="shared" si="0"/>
         <v>66</v>
       </c>
-      <c r="G17" s="11" t="s">
+      <c r="G17" s="23" t="s">
         <v>89</v>
       </c>
-      <c r="H17" s="5" t="s">
+      <c r="H17" s="24" t="s">
         <v>88</v>
       </c>
-      <c r="I17" s="5" t="s">
+      <c r="I17" s="24" t="s">
         <v>90</v>
       </c>
       <c r="J17" t="s">
@@ -1993,7 +2003,7 @@
         <f t="shared" si="0"/>
         <v>8</v>
       </c>
-      <c r="G22" s="3"/>
+      <c r="G22" s="25"/>
       <c r="H22" s="5"/>
     </row>
     <row r="23" spans="1:10" x14ac:dyDescent="0.35">
@@ -2079,8 +2089,15 @@
         <v>122</v>
       </c>
     </row>
+    <row r="29" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="G29" s="10" t="s">
+        <v>124</v>
+      </c>
+    </row>
     <row r="30" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="G30" s="8"/>
+      <c r="G30" s="15" t="s">
+        <v>125</v>
+      </c>
       <c r="H30" s="16"/>
       <c r="I30" s="4"/>
     </row>
@@ -2270,6 +2287,8 @@
     <hyperlink ref="G21" r:id="rId25" xr:uid="{73EBEE48-31EF-41AC-873A-3646DA778705}"/>
     <hyperlink ref="H2" r:id="rId26" xr:uid="{08D83CA7-07B8-4C5F-86A8-BCA2BD2F4632}"/>
     <hyperlink ref="G2" r:id="rId27" display="Battery holder 3xAA" xr:uid="{8C443DA0-0468-4015-B40A-7D52A86ABBE3}"/>
+    <hyperlink ref="G29" r:id="rId28" display="USB - FEMALE, NAT" xr:uid="{ECE2A110-E780-48D1-822E-12AD82DFF7C6}"/>
+    <hyperlink ref="G30" r:id="rId29" display="USB - MALE, NAT" xr:uid="{E124F74D-48FB-4D24-86FA-2CBFB9A2C9C2}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>